<commit_message>
push final mapping file iteration outputs
</commit_message>
<xml_diff>
--- a/termNIT/2023/R_OUT - TERMNIT_mapping_2023-output_from_01.xlsx
+++ b/termNIT/2023/R_OUT - TERMNIT_mapping_2023-output_from_01.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,62 +460,52 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>n_NA</t>
+          <t>n_age_2</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>n_2</t>
+          <t>n_age_3</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>n_3</t>
+          <t>n_age_4</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>n_4</t>
+          <t>n_age_5</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>n_5</t>
+          <t>n_age_6</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>n_6</t>
+          <t>propn_age_2</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>propn_NA</t>
+          <t>propn_age_3</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>propn_2</t>
+          <t>propn_age_4</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>propn_3</t>
+          <t>propn_age_5</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>propn_4</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>propn_5</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>propn_6</t>
+          <t>propn_age_6</t>
         </is>
       </c>
     </row>
@@ -1102,19 +1092,24 @@
           <t>13</t>
         </is>
       </c>
+      <c r="U8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y8" t="inlineStr">
@@ -1127,27 +1122,22 @@
           <t>0</t>
         </is>
       </c>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>0.318181818181818</t>
+        </is>
+      </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.681818181818182</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>0.318181818181818</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
-        <is>
-          <t>0.681818181818182</t>
-        </is>
-      </c>
-      <c r="AE8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AF8" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1244,19 +1234,24 @@
           <t>8</t>
         </is>
       </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
@@ -1269,27 +1264,22 @@
           <t>0</t>
         </is>
       </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>0.318181818181818</t>
+        </is>
+      </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.681818181818182</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>0.318181818181818</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
-        <is>
-          <t>0.681818181818182</t>
-        </is>
-      </c>
-      <c r="AE9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AF9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1386,19 +1376,24 @@
           <t>1</t>
         </is>
       </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y10" t="inlineStr">
@@ -1411,27 +1406,22 @@
           <t>0</t>
         </is>
       </c>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>0.318181818181818</t>
+        </is>
+      </c>
       <c r="AB10" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.681818181818182</t>
         </is>
       </c>
       <c r="AC10" t="inlineStr">
         <is>
-          <t>0.318181818181818</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AD10" t="inlineStr">
-        <is>
-          <t>0.681818181818182</t>
-        </is>
-      </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AF10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1528,19 +1518,24 @@
           <t>0</t>
         </is>
       </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>7</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
@@ -1553,27 +1548,22 @@
           <t>0</t>
         </is>
       </c>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>0.318181818181818</t>
+        </is>
+      </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0.681818181818182</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>0.318181818181818</t>
+          <t>0</t>
         </is>
       </c>
       <c r="AD11" t="inlineStr">
-        <is>
-          <t>0.681818181818182</t>
-        </is>
-      </c>
-      <c r="AE11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AF11" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>